<commit_message>
19CSC45 STATISTICS ASSIGNMENT 1
</commit_message>
<xml_diff>
--- a/19CSC45 SHAMEEMA NAZRIN S STATISTICS.xlsx
+++ b/19CSC45 SHAMEEMA NAZRIN S STATISTICS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shameema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270940FF-EAF2-46F5-9E9B-04ABF42E05E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44671511-9190-41DF-AB82-3C7FF3B65181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E955AD20-7D4A-477F-9778-786D6F4E9AE2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="796">
   <si>
     <t xml:space="preserve"> Arunachal Pradesh</t>
   </si>
@@ -2068,9 +2068,6 @@
   </si>
   <si>
     <t>MIDPOINT</t>
-  </si>
-  <si>
-    <t>CONTINOUS</t>
   </si>
   <si>
     <t>36-42</t>
@@ -2366,9 +2363,6 @@
   </si>
   <si>
     <t>4)MODE</t>
-  </si>
-  <si>
-    <t>FUNTION</t>
   </si>
   <si>
     <t>MODE=</t>
@@ -2666,7 +2660,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2732,6 +2725,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5480,42 +5474,42 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$14:$I$24</c:f>
+              <c:f>Sheet1!$J$14:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>96</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5655,42 +5649,42 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$14:$I$24</c:f>
+              <c:f>Sheet1!$J$14:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>96</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11949,8 +11943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB8A004-379C-43DD-85B2-A6925723DCE4}">
   <dimension ref="A1:S641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G283" workbookViewId="0">
-      <selection activeCell="I170" sqref="I170"/>
+    <sheetView tabSelected="1" topLeftCell="F280" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11986,7 +11980,7 @@
       <c r="D1" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -12099,7 +12093,7 @@
       <c r="D9">
         <v>85.31</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>673</v>
       </c>
       <c r="H9" s="3">
@@ -12129,7 +12123,7 @@
       <c r="D10">
         <v>66.59</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>674</v>
       </c>
       <c r="H10" s="3">
@@ -12205,9 +12199,7 @@
       <c r="M13" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="N13" s="7" t="s">
-        <v>681</v>
-      </c>
+      <c r="N13" s="42"/>
       <c r="P13" s="4" t="s">
         <v>679</v>
       </c>
@@ -12254,7 +12246,7 @@
         <v>640</v>
       </c>
       <c r="P14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Q14" s="1">
         <v>2</v>
@@ -12300,7 +12292,7 @@
         <v>638</v>
       </c>
       <c r="P15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="Q15" s="1">
         <v>4</v>
@@ -12348,7 +12340,7 @@
         <v>634</v>
       </c>
       <c r="P16" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Q16" s="1">
         <v>22</v>
@@ -12396,7 +12388,7 @@
         <v>612</v>
       </c>
       <c r="P17" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="Q17" s="1">
         <v>50</v>
@@ -12444,7 +12436,7 @@
         <v>562</v>
       </c>
       <c r="P18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Q18" s="1">
         <v>97</v>
@@ -12492,7 +12484,7 @@
         <v>465</v>
       </c>
       <c r="P19" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="Q19" s="1">
         <v>140</v>
@@ -12519,19 +12511,19 @@
       <c r="D20">
         <v>70.989999999999995</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>72</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>78</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="12">
         <v>75</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <v>127</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="12">
         <f>FREQUENCY(D2:D641,I20)</f>
         <v>442</v>
       </c>
@@ -12540,7 +12532,7 @@
         <v>325</v>
       </c>
       <c r="P20" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="Q20" s="1">
         <v>127</v>
@@ -12588,7 +12580,7 @@
         <v>198</v>
       </c>
       <c r="P21" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Q21" s="1">
         <v>109</v>
@@ -12636,7 +12628,7 @@
         <v>89</v>
       </c>
       <c r="P22" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="Q22" s="1">
         <v>67</v>
@@ -12684,7 +12676,7 @@
         <v>22</v>
       </c>
       <c r="P23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Q23" s="1">
         <v>17</v>
@@ -12732,7 +12724,7 @@
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="Q24" s="1">
         <v>5</v>
@@ -13781,7 +13773,7 @@
       <c r="D98">
         <v>67.25</v>
       </c>
-      <c r="G98" s="15"/>
+      <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A99">
@@ -13796,8 +13788,8 @@
       <c r="D99">
         <v>63.08</v>
       </c>
-      <c r="H99" s="9" t="s">
-        <v>693</v>
+      <c r="H99" s="8" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -13827,29 +13819,29 @@
       <c r="D101">
         <v>79.06</v>
       </c>
-      <c r="F101" s="18" t="s">
-        <v>719</v>
-      </c>
-      <c r="G101" s="19" t="s">
-        <v>717</v>
-      </c>
-      <c r="H101" s="18">
+      <c r="F101" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>716</v>
+      </c>
+      <c r="H101" s="17">
         <f>AVERAGE(D2:D641)</f>
         <v>72.308421874999965</v>
       </c>
-      <c r="I101" s="41"/>
-      <c r="J101" s="19" t="s">
-        <v>718</v>
-      </c>
-      <c r="K101" s="18">
+      <c r="I101" s="40"/>
+      <c r="J101" s="18" t="s">
+        <v>717</v>
+      </c>
+      <c r="K101" s="17">
         <f>GEOMEAN(D2:D641)</f>
         <v>71.515729396499282</v>
       </c>
-      <c r="L101" s="41"/>
-      <c r="M101" s="19" t="s">
-        <v>716</v>
-      </c>
-      <c r="N101" s="18">
+      <c r="L101" s="40"/>
+      <c r="M101" s="18" t="s">
+        <v>715</v>
+      </c>
+      <c r="N101" s="17">
         <f>HARMEAN(D2:D641)</f>
         <v>70.681256492719072</v>
       </c>
@@ -13937,11 +13929,11 @@
       <c r="D107">
         <v>51.08</v>
       </c>
-      <c r="H107" s="10" t="s">
-        <v>694</v>
-      </c>
-      <c r="L107" s="10" t="s">
-        <v>703</v>
+      <c r="H107" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="L107" s="9" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="108" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13958,31 +13950,31 @@
         <v>61.75</v>
       </c>
       <c r="G108" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="H108" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="H108" s="4" t="s">
+      <c r="I108" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="J108" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="J108" s="4" t="s">
-        <v>698</v>
-      </c>
       <c r="L108" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="M108" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="M108" s="4" t="s">
+      <c r="N108" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="N108" s="4" t="s">
-        <v>697</v>
-      </c>
       <c r="O108" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="P108" s="4" t="s">
         <v>704</v>
-      </c>
-      <c r="P108" s="4" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="109" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13999,7 +13991,7 @@
         <v>70.94</v>
       </c>
       <c r="G109" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H109">
         <v>39</v>
@@ -14012,7 +14004,7 @@
         <v>78</v>
       </c>
       <c r="L109" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M109">
         <v>39</v>
@@ -14043,7 +14035,7 @@
         <v>70.09</v>
       </c>
       <c r="G110" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H110">
         <v>45</v>
@@ -14056,7 +14048,7 @@
         <v>180</v>
       </c>
       <c r="L110" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M110">
         <v>45</v>
@@ -14087,7 +14079,7 @@
         <v>95.08</v>
       </c>
       <c r="G111" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H111">
         <v>51</v>
@@ -14100,7 +14092,7 @@
         <v>1122</v>
       </c>
       <c r="L111" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M111">
         <v>51</v>
@@ -14131,7 +14123,7 @@
         <v>65.319999999999993</v>
       </c>
       <c r="G112" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H112">
         <v>57</v>
@@ -14144,7 +14136,7 @@
         <v>2850</v>
       </c>
       <c r="L112" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="M112">
         <v>57</v>
@@ -14175,7 +14167,7 @@
         <v>66.37</v>
       </c>
       <c r="G113" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H113">
         <v>63</v>
@@ -14188,7 +14180,7 @@
         <v>6111</v>
       </c>
       <c r="L113" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="M113">
         <v>63</v>
@@ -14219,7 +14211,7 @@
         <v>71.13</v>
       </c>
       <c r="G114" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H114">
         <v>69</v>
@@ -14232,7 +14224,7 @@
         <v>9660</v>
       </c>
       <c r="L114" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="M114">
         <v>69</v>
@@ -14263,12 +14255,12 @@
         <v>95.08</v>
       </c>
       <c r="G115" t="s">
-        <v>688</v>
-      </c>
-      <c r="H115" s="13">
+        <v>687</v>
+      </c>
+      <c r="H115" s="12">
         <v>75</v>
       </c>
-      <c r="I115" s="14">
+      <c r="I115" s="13">
         <v>127</v>
       </c>
       <c r="J115">
@@ -14276,12 +14268,12 @@
         <v>9525</v>
       </c>
       <c r="L115" t="s">
-        <v>688</v>
-      </c>
-      <c r="M115" s="13">
+        <v>687</v>
+      </c>
+      <c r="M115" s="12">
         <v>75</v>
       </c>
-      <c r="N115" s="14">
+      <c r="N115" s="13">
         <v>127</v>
       </c>
       <c r="O115">
@@ -14307,7 +14299,7 @@
         <v>89.21</v>
       </c>
       <c r="G116" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H116">
         <v>81</v>
@@ -14320,7 +14312,7 @@
         <v>8829</v>
       </c>
       <c r="L116" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="M116">
         <v>81</v>
@@ -14351,7 +14343,7 @@
         <v>82.5</v>
       </c>
       <c r="G117" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H117">
         <v>87</v>
@@ -14364,7 +14356,7 @@
         <v>5829</v>
       </c>
       <c r="L117" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="M117">
         <v>87</v>
@@ -14395,7 +14387,7 @@
         <v>52.24</v>
       </c>
       <c r="G118" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H118">
         <v>93</v>
@@ -14408,7 +14400,7 @@
         <v>1581</v>
       </c>
       <c r="L118" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="M118">
         <v>93</v>
@@ -14439,7 +14431,7 @@
         <v>61.82</v>
       </c>
       <c r="G119" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H119">
         <v>99</v>
@@ -14452,7 +14444,7 @@
         <v>495</v>
       </c>
       <c r="L119" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="M119">
         <v>99</v>
@@ -14483,7 +14475,7 @@
         <v>83.45</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I120" s="5">
         <f>SUM(I109:I119)</f>
@@ -14494,7 +14486,7 @@
         <v>46260</v>
       </c>
       <c r="M120" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N120" s="5">
         <f>SUM(N109:N119)</f>
@@ -14520,10 +14512,10 @@
         <v>63.14</v>
       </c>
       <c r="H121" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="M121" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
@@ -14540,10 +14532,10 @@
         <v>61.42</v>
       </c>
       <c r="H122" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="M122" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="123" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -14559,15 +14551,15 @@
       <c r="D123">
         <v>59.07</v>
       </c>
-      <c r="G123" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="H123" s="12">
+      <c r="G123" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="H123" s="11">
         <f>J120/I120</f>
         <v>72.28125</v>
       </c>
-      <c r="L123" s="15" t="s">
-        <v>708</v>
+      <c r="L123" s="14" t="s">
+        <v>707</v>
       </c>
       <c r="M123">
         <f>P120/N120</f>
@@ -14588,7 +14580,7 @@
         <v>59.54</v>
       </c>
       <c r="M124" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="125" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -14604,10 +14596,10 @@
       <c r="D125">
         <v>82.87</v>
       </c>
-      <c r="L125" s="12" t="s">
-        <v>710</v>
-      </c>
-      <c r="M125" s="12">
+      <c r="L125" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="M125" s="11">
         <f>POWER(10,M123)</f>
         <v>71.479971044212448</v>
       </c>
@@ -14639,8 +14631,8 @@
       <c r="D127">
         <v>63.87</v>
       </c>
-      <c r="G127" s="10" t="s">
-        <v>711</v>
+      <c r="G127" s="9" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -14699,16 +14691,16 @@
         <v>76.06</v>
       </c>
       <c r="G131" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="H131" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="H131" s="4" t="s">
+      <c r="I131" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="I131" s="4" t="s">
-        <v>697</v>
-      </c>
       <c r="J131" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="132" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14725,7 +14717,7 @@
         <v>87.38</v>
       </c>
       <c r="G132" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H132">
         <v>39</v>
@@ -14752,7 +14744,7 @@
         <v>67.3</v>
       </c>
       <c r="G133" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H133">
         <v>45</v>
@@ -14779,7 +14771,7 @@
         <v>75.52</v>
       </c>
       <c r="G134" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H134">
         <v>51</v>
@@ -14806,7 +14798,7 @@
         <v>64.430000000000007</v>
       </c>
       <c r="G135" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H135">
         <v>57</v>
@@ -14833,7 +14825,7 @@
         <v>72.37</v>
       </c>
       <c r="G136" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H136">
         <v>63</v>
@@ -14860,7 +14852,7 @@
         <v>81.48</v>
       </c>
       <c r="G137" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H137">
         <v>69</v>
@@ -14887,12 +14879,12 @@
         <v>74.78</v>
       </c>
       <c r="G138" t="s">
-        <v>688</v>
-      </c>
-      <c r="H138" s="13">
+        <v>687</v>
+      </c>
+      <c r="H138" s="12">
         <v>75</v>
       </c>
-      <c r="I138" s="14">
+      <c r="I138" s="13">
         <v>127</v>
       </c>
       <c r="J138">
@@ -14914,7 +14906,7 @@
         <v>53.53</v>
       </c>
       <c r="G139" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H139">
         <v>81</v>
@@ -14941,7 +14933,7 @@
         <v>89.31</v>
       </c>
       <c r="G140" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H140">
         <v>87</v>
@@ -14968,7 +14960,7 @@
         <v>64.81</v>
       </c>
       <c r="G141" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H141">
         <v>93</v>
@@ -14995,7 +14987,7 @@
         <v>82.82</v>
       </c>
       <c r="G142" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H142">
         <v>99</v>
@@ -15022,7 +15014,7 @@
         <v>75.8</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I143" s="5">
         <f>SUM(I132:I142)</f>
@@ -15047,7 +15039,7 @@
         <v>61.01</v>
       </c>
       <c r="H144" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -15064,7 +15056,7 @@
         <v>86.57</v>
       </c>
       <c r="H145" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -15080,7 +15072,7 @@
       <c r="D146">
         <v>70.47</v>
       </c>
-      <c r="H146" s="16">
+      <c r="H146" s="15">
         <f>J143/I143</f>
         <v>1.4155988369083022E-2</v>
       </c>
@@ -15099,7 +15091,7 @@
         <v>83.23</v>
       </c>
       <c r="H147" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -15115,10 +15107,10 @@
       <c r="D148">
         <v>61.74</v>
       </c>
-      <c r="G148" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="H148" s="12">
+      <c r="G148" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="H148" s="11">
         <f>1/H146</f>
         <v>70.641482171885727</v>
       </c>
@@ -15164,8 +15156,8 @@
       <c r="D151">
         <v>75.14</v>
       </c>
-      <c r="G151" s="10" t="s">
-        <v>720</v>
+      <c r="G151" s="9" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -15195,13 +15187,13 @@
       <c r="D153">
         <v>70.78</v>
       </c>
-      <c r="F153" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="G153" s="17" t="s">
-        <v>721</v>
-      </c>
-      <c r="H153" s="8">
+      <c r="F153" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="G153" s="16" t="s">
+        <v>720</v>
+      </c>
+      <c r="H153" s="7">
         <f>MEDIAN(D2:D641)</f>
         <v>72.17</v>
       </c>
@@ -15276,13 +15268,13 @@
         <v>78.040000000000006</v>
       </c>
       <c r="G158" s="4" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H158" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I158" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15299,7 +15291,7 @@
         <v>56.53</v>
       </c>
       <c r="G159" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H159" s="1">
         <v>2</v>
@@ -15322,7 +15314,7 @@
         <v>83.4</v>
       </c>
       <c r="G160" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H160" s="1">
         <v>4</v>
@@ -15346,7 +15338,7 @@
         <v>76.989999999999995</v>
       </c>
       <c r="G161" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H161" s="1">
         <v>22</v>
@@ -15356,7 +15348,7 @@
         <v>28</v>
       </c>
       <c r="L161" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="162" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15373,7 +15365,7 @@
         <v>69.33</v>
       </c>
       <c r="G162" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H162" s="1">
         <v>50</v>
@@ -15383,7 +15375,7 @@
         <v>78</v>
       </c>
       <c r="L162" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15400,7 +15392,7 @@
         <v>64.849999999999994</v>
       </c>
       <c r="G163" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H163" s="1">
         <v>97</v>
@@ -15424,7 +15416,7 @@
         <v>65.47</v>
       </c>
       <c r="G164" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H164" s="1">
         <v>140</v>
@@ -15433,11 +15425,11 @@
         <f t="shared" si="8"/>
         <v>315</v>
       </c>
-      <c r="K164" s="20" t="s">
-        <v>723</v>
-      </c>
-      <c r="L164" s="20" t="s">
-        <v>737</v>
+      <c r="K164" s="19" t="s">
+        <v>722</v>
+      </c>
+      <c r="L164" s="19" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="165" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15453,21 +15445,21 @@
       <c r="D165">
         <v>59.25</v>
       </c>
-      <c r="G165" s="22" t="s">
-        <v>688</v>
-      </c>
-      <c r="H165" s="23">
+      <c r="G165" s="21" t="s">
+        <v>687</v>
+      </c>
+      <c r="H165" s="22">
         <v>127</v>
       </c>
-      <c r="I165" s="22">
+      <c r="I165" s="21">
         <f t="shared" si="8"/>
         <v>442</v>
       </c>
-      <c r="J165" s="22" t="s">
-        <v>731</v>
+      <c r="J165" s="21" t="s">
+        <v>730</v>
       </c>
       <c r="L165" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="166" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15484,7 +15476,7 @@
         <v>61.25</v>
       </c>
       <c r="G166" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H166" s="1">
         <v>109</v>
@@ -15494,7 +15486,7 @@
         <v>551</v>
       </c>
       <c r="L166" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="167" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15511,7 +15503,7 @@
         <v>70.11</v>
       </c>
       <c r="G167" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H167" s="1">
         <v>67</v>
@@ -15521,7 +15513,7 @@
         <v>618</v>
       </c>
       <c r="L167" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="168" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15538,7 +15530,7 @@
         <v>70.36</v>
       </c>
       <c r="G168" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H168" s="1">
         <v>17</v>
@@ -15548,7 +15540,7 @@
         <v>635</v>
       </c>
       <c r="L168" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15565,7 +15557,7 @@
         <v>86.98</v>
       </c>
       <c r="G169" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H169" s="1">
         <v>5</v>
@@ -15575,7 +15567,7 @@
         <v>640</v>
       </c>
       <c r="L169" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="170" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -15592,16 +15584,16 @@
         <v>70.319999999999993</v>
       </c>
       <c r="G170" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H170" s="5">
         <f>SUM(H159:H169)</f>
         <v>640</v>
       </c>
-      <c r="L170" s="12" t="s">
-        <v>721</v>
-      </c>
-      <c r="M170" s="21">
+      <c r="L170" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="M170" s="20">
         <v>72.23</v>
       </c>
     </row>
@@ -15632,8 +15624,8 @@
       <c r="D172">
         <v>63.17</v>
       </c>
-      <c r="G172" s="10" t="s">
-        <v>732</v>
+      <c r="G172" s="9" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -15706,19 +15698,19 @@
         <v>68.73</v>
       </c>
       <c r="G177" s="4" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H177" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I177" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="J177" s="19" t="s">
         <v>722</v>
       </c>
-      <c r="J177" s="20" t="s">
-        <v>723</v>
-      </c>
-      <c r="K177" s="20" t="s">
-        <v>733</v>
+      <c r="K177" s="19" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15735,7 +15727,7 @@
         <v>74.209999999999994</v>
       </c>
       <c r="G178" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H178" s="1">
         <v>2</v>
@@ -15744,7 +15736,7 @@
         <v>2</v>
       </c>
       <c r="K178" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="179" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15761,7 +15753,7 @@
         <v>67.22</v>
       </c>
       <c r="G179" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H179" s="1">
         <v>4</v>
@@ -15771,7 +15763,7 @@
         <v>6</v>
       </c>
       <c r="K179" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="180" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15788,7 +15780,7 @@
         <v>81.069999999999993</v>
       </c>
       <c r="G180" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H180" s="1">
         <v>22</v>
@@ -15798,10 +15790,10 @@
         <v>28</v>
       </c>
       <c r="L180" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="M180" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="181" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15818,7 +15810,7 @@
         <v>77.260000000000005</v>
       </c>
       <c r="G181" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H181" s="1">
         <v>50</v>
@@ -15841,27 +15833,27 @@
       <c r="D182">
         <v>67.430000000000007</v>
       </c>
-      <c r="G182" s="24" t="s">
-        <v>686</v>
-      </c>
-      <c r="H182" s="25">
+      <c r="G182" s="23" t="s">
+        <v>685</v>
+      </c>
+      <c r="H182" s="24">
         <v>97</v>
       </c>
-      <c r="I182" s="24">
+      <c r="I182" s="23">
         <f t="shared" si="9"/>
         <v>175</v>
       </c>
       <c r="J182" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K182" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="L182" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M182" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="183" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15878,7 +15870,7 @@
         <v>63.14</v>
       </c>
       <c r="G183" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H183" s="1">
         <v>140</v>
@@ -15888,13 +15880,13 @@
         <v>315</v>
       </c>
       <c r="K183" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="L183" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="M183" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="184" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15910,27 +15902,27 @@
       <c r="D184">
         <v>75.790000000000006</v>
       </c>
-      <c r="G184" s="22" t="s">
-        <v>688</v>
-      </c>
-      <c r="H184" s="23">
+      <c r="G184" s="21" t="s">
+        <v>687</v>
+      </c>
+      <c r="H184" s="22">
         <v>127</v>
       </c>
-      <c r="I184" s="22">
+      <c r="I184" s="21">
         <f t="shared" si="9"/>
         <v>442</v>
       </c>
       <c r="J184" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="K184" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="L184" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="M184" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="185" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15946,24 +15938,24 @@
       <c r="D185">
         <v>61.37</v>
       </c>
-      <c r="G185" s="27" t="s">
-        <v>689</v>
-      </c>
-      <c r="H185" s="28">
+      <c r="G185" s="26" t="s">
+        <v>688</v>
+      </c>
+      <c r="H185" s="27">
         <v>109</v>
       </c>
-      <c r="I185" s="27">
+      <c r="I185" s="26">
         <f t="shared" si="9"/>
         <v>551</v>
       </c>
       <c r="K185" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L185" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="M185" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="186" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15980,7 +15972,7 @@
         <v>82.64</v>
       </c>
       <c r="G186" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H186" s="1">
         <v>67</v>
@@ -15990,13 +15982,13 @@
         <v>618</v>
       </c>
       <c r="K186" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L186" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="M186" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="187" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16013,7 +16005,7 @@
         <v>72.23</v>
       </c>
       <c r="G187" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H187" s="1">
         <v>17</v>
@@ -16022,14 +16014,14 @@
         <f t="shared" si="9"/>
         <v>635</v>
       </c>
-      <c r="K187" s="24" t="s">
-        <v>743</v>
-      </c>
-      <c r="L187" s="22" t="s">
-        <v>751</v>
-      </c>
-      <c r="M187" s="27" t="s">
-        <v>760</v>
+      <c r="K187" s="23" t="s">
+        <v>742</v>
+      </c>
+      <c r="L187" s="21" t="s">
+        <v>750</v>
+      </c>
+      <c r="M187" s="26" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="188" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16046,7 +16038,7 @@
         <v>70.989999999999995</v>
       </c>
       <c r="G188" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H188" s="1">
         <v>5</v>
@@ -16055,8 +16047,8 @@
         <f t="shared" si="9"/>
         <v>640</v>
       </c>
-      <c r="L188" s="22" t="s">
-        <v>745</v>
+      <c r="L188" s="21" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -16073,20 +16065,20 @@
         <v>76.459999999999994</v>
       </c>
       <c r="G189" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H189" s="5">
         <f>SUM(H178:H188)</f>
         <v>640</v>
       </c>
-      <c r="K189" s="24" t="s">
-        <v>742</v>
-      </c>
-      <c r="L189" s="22" t="s">
-        <v>746</v>
-      </c>
-      <c r="M189" s="27" t="s">
-        <v>753</v>
+      <c r="K189" s="23" t="s">
+        <v>741</v>
+      </c>
+      <c r="L189" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="M189" s="26" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -16145,17 +16137,17 @@
         <v>60.01</v>
       </c>
       <c r="J193" s="2"/>
-      <c r="K193" s="29" t="s">
+      <c r="K193" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="L193" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="L193" s="29" t="s">
+      <c r="M193" s="28" t="s">
         <v>762</v>
       </c>
-      <c r="M193" s="29" t="s">
+      <c r="N193" s="28" t="s">
         <v>763</v>
-      </c>
-      <c r="N193" s="29" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
@@ -16172,21 +16164,21 @@
         <v>58.89</v>
       </c>
       <c r="J194" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="K194" s="29">
+        <v>718</v>
+      </c>
+      <c r="K194" s="28">
         <f>QUARTILE(D2:D641,1)</f>
         <v>65.094999999999999</v>
       </c>
-      <c r="L194" s="29">
+      <c r="L194" s="28">
         <f>QUARTILE(D2:D641,2)</f>
         <v>72.17</v>
       </c>
-      <c r="M194" s="29">
+      <c r="M194" s="28">
         <f>QUARTILE(D2:D641,3)</f>
         <v>79.962500000000006</v>
       </c>
-      <c r="N194" s="29">
+      <c r="N194" s="28">
         <f>QUARTILE(D2:D641,4)</f>
         <v>97.91</v>
       </c>
@@ -16250,8 +16242,8 @@
       <c r="D198">
         <v>79.95</v>
       </c>
-      <c r="G198" s="10" t="s">
-        <v>765</v>
+      <c r="G198" s="9" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
@@ -16310,10 +16302,10 @@
         <v>86.88</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="H202" s="31" t="s">
-        <v>767</v>
+        <v>787</v>
+      </c>
+      <c r="H202" s="30" t="s">
+        <v>765</v>
       </c>
       <c r="I202" s="2">
         <f>MODE(D2:D641)</f>
@@ -16361,11 +16353,11 @@
       <c r="D205">
         <v>72.260000000000005</v>
       </c>
-      <c r="G205" s="32" t="s">
-        <v>695</v>
-      </c>
-      <c r="H205" s="32" t="s">
-        <v>697</v>
+      <c r="G205" s="31" t="s">
+        <v>694</v>
+      </c>
+      <c r="H205" s="31" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="206" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16382,16 +16374,16 @@
         <v>59.76</v>
       </c>
       <c r="G206" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H206" s="1">
         <v>2</v>
       </c>
-      <c r="J206" s="26" t="s">
-        <v>768</v>
-      </c>
-      <c r="K206" s="26" t="s">
-        <v>769</v>
+      <c r="J206" s="25" t="s">
+        <v>766</v>
+      </c>
+      <c r="K206" s="25" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="207" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16408,7 +16400,7 @@
         <v>73.09</v>
       </c>
       <c r="G207" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H207" s="1">
         <v>4</v>
@@ -16428,13 +16420,13 @@
         <v>80.010000000000005</v>
       </c>
       <c r="G208" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H208" s="1">
         <v>22</v>
       </c>
       <c r="J208" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="209" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16451,13 +16443,13 @@
         <v>82.48</v>
       </c>
       <c r="G209" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H209" s="1">
         <v>50</v>
       </c>
       <c r="J209" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="210" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16474,13 +16466,13 @@
         <v>59</v>
       </c>
       <c r="G210" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H210" s="1">
         <v>97</v>
       </c>
       <c r="J210" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="211" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16496,17 +16488,17 @@
       <c r="D211">
         <v>67.150000000000006</v>
       </c>
-      <c r="G211" s="34" t="s">
-        <v>687</v>
-      </c>
-      <c r="H211" s="35">
+      <c r="G211" s="33" t="s">
+        <v>686</v>
+      </c>
+      <c r="H211" s="34">
         <v>140</v>
       </c>
       <c r="I211" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="J211" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="212" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16523,13 +16515,13 @@
         <v>73.650000000000006</v>
       </c>
       <c r="G212" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H212" s="1">
         <v>127</v>
       </c>
       <c r="J212" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="213" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -16546,13 +16538,13 @@
         <v>76.260000000000005</v>
       </c>
       <c r="G213" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H213" s="1">
         <v>109</v>
       </c>
-      <c r="J213" s="33" t="s">
-        <v>774</v>
+      <c r="J213" s="32" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="214" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16569,7 +16561,7 @@
         <v>49.51</v>
       </c>
       <c r="G214" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H214" s="1">
         <v>67</v>
@@ -16589,7 +16581,7 @@
         <v>74.13</v>
       </c>
       <c r="G215" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H215" s="1">
         <v>17</v>
@@ -16609,7 +16601,7 @@
         <v>95.72</v>
       </c>
       <c r="G216" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H216" s="1">
         <v>5</v>
@@ -16796,8 +16788,8 @@
       <c r="D229">
         <v>76.650000000000006</v>
       </c>
-      <c r="H229" s="10" t="s">
-        <v>775</v>
+      <c r="H229" s="9" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="230" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -16813,23 +16805,23 @@
       <c r="D230">
         <v>61.47</v>
       </c>
-      <c r="G230" s="32" t="s">
-        <v>695</v>
-      </c>
-      <c r="H230" s="32" t="s">
+      <c r="G230" s="31" t="s">
+        <v>694</v>
+      </c>
+      <c r="H230" s="31" t="s">
+        <v>774</v>
+      </c>
+      <c r="I230" s="31" t="s">
+        <v>696</v>
+      </c>
+      <c r="J230" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="K230" s="31" t="s">
         <v>776</v>
       </c>
-      <c r="I230" s="32" t="s">
-        <v>697</v>
-      </c>
-      <c r="J230" s="4" t="s">
+      <c r="L230" s="31" t="s">
         <v>777</v>
-      </c>
-      <c r="K230" s="32" t="s">
-        <v>778</v>
-      </c>
-      <c r="L230" s="32" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16846,7 +16838,7 @@
         <v>68.92</v>
       </c>
       <c r="G231" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H231">
         <v>39</v>
@@ -16881,7 +16873,7 @@
         <v>52.25</v>
       </c>
       <c r="G232" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H232">
         <v>45</v>
@@ -16916,7 +16908,7 @@
         <v>75.05</v>
       </c>
       <c r="G233" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H233">
         <v>51</v>
@@ -16951,7 +16943,7 @@
         <v>72.34</v>
       </c>
       <c r="G234" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H234">
         <v>57</v>
@@ -16986,7 +16978,7 @@
         <v>97.21</v>
       </c>
       <c r="G235" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H235">
         <v>63</v>
@@ -17021,7 +17013,7 @@
         <v>69.64</v>
       </c>
       <c r="G236" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H236">
         <v>69</v>
@@ -17056,12 +17048,12 @@
         <v>71.03</v>
       </c>
       <c r="G237" t="s">
-        <v>688</v>
-      </c>
-      <c r="H237" s="13">
+        <v>687</v>
+      </c>
+      <c r="H237" s="12">
         <v>75</v>
       </c>
-      <c r="I237" s="14">
+      <c r="I237" s="13">
         <v>127</v>
       </c>
       <c r="J237">
@@ -17091,7 +17083,7 @@
         <v>71.52</v>
       </c>
       <c r="G238" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H238">
         <v>81</v>
@@ -17126,7 +17118,7 @@
         <v>71.48</v>
       </c>
       <c r="G239" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H239">
         <v>87</v>
@@ -17161,7 +17153,7 @@
         <v>76.56</v>
       </c>
       <c r="G240" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H240">
         <v>93</v>
@@ -17196,7 +17188,7 @@
         <v>58.34</v>
       </c>
       <c r="G241" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H241">
         <v>99</v>
@@ -17231,7 +17223,7 @@
         <v>75.739999999999995</v>
       </c>
       <c r="H242" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I242" s="5">
         <f>SUM(I231:I241)</f>
@@ -17272,13 +17264,13 @@
         <v>63.63</v>
       </c>
       <c r="G244" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H244" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="J244" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -17295,7 +17287,7 @@
         <v>59.56</v>
       </c>
       <c r="H245" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="246" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -17311,8 +17303,8 @@
       <c r="D246">
         <v>67.34</v>
       </c>
-      <c r="I246" s="36" t="s">
-        <v>784</v>
+      <c r="I246" s="35" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -17342,10 +17334,10 @@
       <c r="D248">
         <v>75.28</v>
       </c>
-      <c r="H248" s="21" t="s">
-        <v>782</v>
-      </c>
-      <c r="I248" s="21">
+      <c r="H248" s="20" t="s">
+        <v>780</v>
+      </c>
+      <c r="I248" s="20">
         <f>L242/I242</f>
         <v>111.40874999999998</v>
       </c>
@@ -17377,13 +17369,13 @@
       <c r="D250">
         <v>68.819999999999993</v>
       </c>
-      <c r="G250" s="39" t="s">
-        <v>789</v>
-      </c>
-      <c r="H250" s="40" t="s">
-        <v>782</v>
-      </c>
-      <c r="I250" s="39">
+      <c r="G250" s="38" t="s">
+        <v>787</v>
+      </c>
+      <c r="H250" s="39" t="s">
+        <v>780</v>
+      </c>
+      <c r="I250" s="38">
         <f>_xlfn.VAR.S(D2:D641)</f>
         <v>110.01525243520095</v>
       </c>
@@ -17429,8 +17421,8 @@
       <c r="D253">
         <v>62.7</v>
       </c>
-      <c r="G253" s="37" t="s">
-        <v>785</v>
+      <c r="G253" s="36" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
@@ -17460,11 +17452,11 @@
       <c r="D255">
         <v>75.989999999999995</v>
       </c>
-      <c r="G255" s="26" t="s">
-        <v>723</v>
-      </c>
-      <c r="H255" s="38" t="s">
-        <v>786</v>
+      <c r="G255" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="H255" s="37" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
@@ -17509,7 +17501,7 @@
         <v>79.56</v>
       </c>
       <c r="G258" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="259" spans="1:10" ht="21" x14ac:dyDescent="0.35">
@@ -17525,10 +17517,10 @@
       <c r="D259">
         <v>63.84</v>
       </c>
-      <c r="G259" s="37" t="s">
-        <v>787</v>
-      </c>
-      <c r="H259" s="37">
+      <c r="G259" s="36" t="s">
+        <v>785</v>
+      </c>
+      <c r="H259" s="36">
         <f>SQRT(I248)</f>
         <v>10.555034343856963</v>
       </c>
@@ -17560,13 +17552,13 @@
       <c r="D261">
         <v>54.86</v>
       </c>
-      <c r="G261" s="39" t="s">
-        <v>789</v>
-      </c>
-      <c r="H261" s="40" t="s">
+      <c r="G261" s="38" t="s">
         <v>787</v>
       </c>
-      <c r="I261" s="39">
+      <c r="H261" s="39" t="s">
+        <v>785</v>
+      </c>
+      <c r="I261" s="38">
         <f>_xlfn.STDEV.S(D2:D641)</f>
         <v>10.488815587815479</v>
       </c>
@@ -17612,8 +17604,8 @@
       <c r="D264">
         <v>81.7</v>
       </c>
-      <c r="G264" s="9" t="s">
-        <v>790</v>
+      <c r="G264" s="8" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
@@ -17644,7 +17636,7 @@
         <v>68.239999999999995</v>
       </c>
       <c r="H266" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
@@ -17674,8 +17666,8 @@
       <c r="D268">
         <v>56.33</v>
       </c>
-      <c r="H268" s="42" t="s">
-        <v>792</v>
+      <c r="H268" s="41" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="269" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -17691,8 +17683,8 @@
       <c r="D269">
         <v>75.78</v>
       </c>
-      <c r="H269" s="21" t="s">
-        <v>694</v>
+      <c r="H269" s="20" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="270" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -17709,16 +17701,16 @@
         <v>76.069999999999993</v>
       </c>
       <c r="G270" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="H270" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="H270" s="4" t="s">
+      <c r="I270" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="I270" s="4" t="s">
+      <c r="J270" s="4" t="s">
         <v>697</v>
-      </c>
-      <c r="J270" s="4" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="271" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17735,7 +17727,7 @@
         <v>67.13</v>
       </c>
       <c r="G271" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H271">
         <v>39</v>
@@ -17762,7 +17754,7 @@
         <v>70.81</v>
       </c>
       <c r="G272" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H272">
         <v>45</v>
@@ -17789,7 +17781,7 @@
         <v>63.74</v>
       </c>
       <c r="G273" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H273">
         <v>51</v>
@@ -17816,7 +17808,7 @@
         <v>59.79</v>
       </c>
       <c r="G274" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H274">
         <v>57</v>
@@ -17843,7 +17835,7 @@
         <v>72.13</v>
       </c>
       <c r="G275" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H275">
         <v>63</v>
@@ -17870,7 +17862,7 @@
         <v>80.45</v>
       </c>
       <c r="G276" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H276">
         <v>69</v>
@@ -17897,12 +17889,12 @@
         <v>86.16</v>
       </c>
       <c r="G277" t="s">
-        <v>688</v>
-      </c>
-      <c r="H277" s="13">
+        <v>687</v>
+      </c>
+      <c r="H277" s="12">
         <v>75</v>
       </c>
-      <c r="I277" s="14">
+      <c r="I277" s="13">
         <v>127</v>
       </c>
       <c r="J277">
@@ -17924,7 +17916,7 @@
         <v>72.89</v>
       </c>
       <c r="G278" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H278">
         <v>81</v>
@@ -17951,7 +17943,7 @@
         <v>79.34</v>
       </c>
       <c r="G279" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H279">
         <v>87</v>
@@ -17978,7 +17970,7 @@
         <v>69.75</v>
       </c>
       <c r="G280" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H280">
         <v>93</v>
@@ -18005,7 +17997,7 @@
         <v>74.63</v>
       </c>
       <c r="G281" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H281">
         <v>99</v>
@@ -18032,7 +18024,7 @@
         <v>62.55</v>
       </c>
       <c r="H282" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I282" s="5">
         <f>SUM(I271:I281)</f>
@@ -18057,7 +18049,7 @@
         <v>88.69</v>
       </c>
       <c r="H283" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
@@ -18074,7 +18066,7 @@
         <v>66.72</v>
       </c>
       <c r="H284" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="285" spans="1:11" ht="21" x14ac:dyDescent="0.35">
@@ -18090,17 +18082,17 @@
       <c r="D285">
         <v>89.31</v>
       </c>
-      <c r="G285" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="H285" s="12">
+      <c r="G285" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="H285" s="11">
         <f>J282/I282</f>
         <v>72.28125</v>
       </c>
-      <c r="J285" s="37" t="s">
-        <v>787</v>
-      </c>
-      <c r="K285" s="37">
+      <c r="J285" s="36" t="s">
+        <v>785</v>
+      </c>
+      <c r="K285" s="36">
         <f>SQRT(I248)</f>
         <v>10.555034343856963</v>
       </c>
@@ -18147,7 +18139,7 @@
         <v>70.510000000000005</v>
       </c>
       <c r="I288" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
@@ -18164,7 +18156,7 @@
         <v>75.260000000000005</v>
       </c>
       <c r="I289" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="290" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -18180,11 +18172,11 @@
       <c r="D290">
         <v>77.09</v>
       </c>
-      <c r="H290" s="21" t="s">
-        <v>793</v>
-      </c>
-      <c r="I290" s="21" t="s">
-        <v>796</v>
+      <c r="H290" s="20" t="s">
+        <v>791</v>
+      </c>
+      <c r="I290" s="20" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
@@ -18214,13 +18206,13 @@
       <c r="D292">
         <v>84.25</v>
       </c>
-      <c r="G292" s="39" t="s">
-        <v>789</v>
-      </c>
-      <c r="H292" s="40" t="s">
-        <v>797</v>
-      </c>
-      <c r="I292" s="39">
+      <c r="G292" s="38" t="s">
+        <v>787</v>
+      </c>
+      <c r="H292" s="39" t="s">
+        <v>795</v>
+      </c>
+      <c r="I292" s="38">
         <f>_xlfn.STDEV.S(D2:D641)/AVERAGE(D2:D641)*100</f>
         <v>14.505662432997863</v>
       </c>

</xml_diff>